<commit_message>
sina and iranzamin is done
</commit_message>
<xml_diff>
--- a/Python/Iranian_Banks.xlsx
+++ b/Python/Iranian_Banks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programming_Practice\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A685FB6-C378-4757-A11A-2F17C650B844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425A6934-FDD4-4ABE-B098-22F2051476AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="106">
   <si>
     <t>Bank Name</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>khavarmianeh_bank_branches_20241115</t>
+  </si>
+  <si>
+    <t>iranzamin_bank_branches_20241117</t>
+  </si>
+  <si>
+    <t>sina_bank_branches_20241117</t>
   </si>
 </sst>
 </file>
@@ -731,7 +737,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1058,17 +1064,19 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
+      <c r="C21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1107,34 +1115,36 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
+      <c r="C24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sina bank data is added
</commit_message>
<xml_diff>
--- a/Python/Iranian_Banks.xlsx
+++ b/Python/Iranian_Banks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasma\Desktop\Kasma_Programming_Practice\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425A6934-FDD4-4ABE-B098-22F2051476AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4174BCBC-08D0-4B6F-86FB-A548DCC0A0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="107">
   <si>
     <t>Bank Name</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>sina_bank_branches_20241117</t>
+  </si>
+  <si>
+    <t>saman_bank_branches_20241119</t>
   </si>
 </sst>
 </file>
@@ -358,7 +361,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,12 +377,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -425,7 +422,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -737,7 +733,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,17 +825,19 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>65</v>
       </c>
     </row>
@@ -998,17 +996,17 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
+      <c r="C17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1064,19 +1062,19 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1115,19 +1113,19 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>